<commit_message>
narisal par prostorskih grafov
</commit_message>
<xml_diff>
--- a/podatki/lokacije.xlsx
+++ b/podatki/lokacije.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b659fc1f114388/Dokumenti/APPR-2021-22/podatki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{202FD741-8745-4EBA-87F4-88EDEC72331A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{202FD741-8745-4EBA-87F4-88EDEC72331A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{776B4E7B-EBA1-49CC-8CAB-E6F364BD1952}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Murska Sobota</t>
   </si>
   <si>
-    <t>Novo Mesto</t>
-  </si>
-  <si>
     <t>Portorož</t>
   </si>
   <si>
@@ -103,12 +100,15 @@
   </si>
   <si>
     <t xml:space="preserve">Velenje </t>
+  </si>
+  <si>
+    <t>Novo mesto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -458,11 +458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +615,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>15.177300000000001</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>13.616</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>14.193199999999999</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>13.712899999999999</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>15.638</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
         <v>13.9354</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>15.1112</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>15.114800000000001</v>

</xml_diff>